<commit_message>
upraven seznam účastníků prezentace, přidány otázky a témata do diskuze
</commit_message>
<xml_diff>
--- a/src/Myrtha_Pools/180314_prezentace_v_prostejove/seznam_ucastniku.xlsx
+++ b/src/Myrtha_Pools/180314_prezentace_v_prostejove/seznam_ucastniku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="0" windowWidth="10740" windowHeight="4140"/>
+    <workbookView xWindow="7650" yWindow="0" windowWidth="10740" windowHeight="4140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -646,7 +646,7 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(G4:G100)</f>
-        <v>13.3</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="27.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>14</v>
@@ -839,9 +839,6 @@
         <v>11</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:7" ht="27.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
Situace pro znázornění velikosti a prostorových možností budoucího sportovního areálu Krasice Skica
</commit_message>
<xml_diff>
--- a/src/Myrtha_Pools/180314_prezentace_v_prostejove/seznam_ucastniku.xlsx
+++ b/src/Myrtha_Pools/180314_prezentace_v_prostejove/seznam_ucastniku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7650" yWindow="0" windowWidth="10740" windowHeight="4140"/>
+    <workbookView xWindow="9180" yWindow="0" windowWidth="10740" windowHeight="4140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="73">
   <si>
     <t>Augustin Josef, JUDr.</t>
   </si>
@@ -152,15 +152,9 @@
     <t>člen zastupitelstva města Prostějov</t>
   </si>
   <si>
-    <t>odborná veřejnost</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>zájem</t>
-  </si>
-  <si>
     <t>Adamec Petr</t>
   </si>
   <si>
@@ -200,20 +194,79 @@
     <t>City municipal council member</t>
   </si>
   <si>
-    <t>Experts</t>
-  </si>
-  <si>
     <t>City municipal council member, 1st Deputy Mayor</t>
   </si>
   <si>
     <t>člen zastupitelstva města Prostějov, 1. náměstek primátora</t>
+  </si>
+  <si>
+    <t>confirmed</t>
+  </si>
+  <si>
+    <t>may come</t>
+  </si>
+  <si>
+    <t>City municipal council member
+member of Senate of the Czech Republic</t>
+  </si>
+  <si>
+    <t>člen zastupitelstva města Prostějov
+člen Senátu Parlamentu ČR</t>
+  </si>
+  <si>
+    <t>City municipal council member
+Head of TJ Prostejov, local sports organization</t>
+  </si>
+  <si>
+    <t>člen zastupitelstva města Prostějov
+předseda sportovní organizace TJ Prostějov</t>
+  </si>
+  <si>
+    <t>City municipal council member
+Elementary school director</t>
+  </si>
+  <si>
+    <t>člen zastupitelstva města Prostějov
+Ředitel základní školy</t>
+  </si>
+  <si>
+    <t>City municipal council member,
+Architect</t>
+  </si>
+  <si>
+    <t>člen zastupitelstva města Prostějov,
+architekt</t>
+  </si>
+  <si>
+    <t>člen zastupitelstva města Prostějov,
+inženýr technického zařízení budov</t>
+  </si>
+  <si>
+    <t>City municipal council member,
+Technical Building Equipment engineer</t>
+  </si>
+  <si>
+    <t>City municipal council member
+economy and management, teacher</t>
+  </si>
+  <si>
+    <t>člen zastupitelstva města Prostějov,
+učitel SŠ, ekonomie a management</t>
+  </si>
+  <si>
+    <t>odborná veřejnost,
+systémový inženýr v letectví</t>
+  </si>
+  <si>
+    <t>Experts,
+system engineer in aeronautics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +293,14 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -293,10 +354,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -327,8 +389,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -608,17 +674,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:H48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="32.85546875" customWidth="1"/>
     <col min="5" max="5" width="28.42578125" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
@@ -626,23 +692,34 @@
     <col min="8" max="8" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
         <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
       </c>
       <c r="G3" s="5">
         <f>SUM(G4:G100)</f>
@@ -651,17 +728,17 @@
     </row>
     <row r="4" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="4">
@@ -674,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>40</v>
@@ -684,13 +761,13 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="27.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>40</v>
@@ -703,13 +780,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="27.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>40</v>
@@ -728,7 +805,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>40</v>
@@ -744,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>40</v>
@@ -760,7 +837,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>40</v>
@@ -776,26 +853,26 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>11</v>
@@ -811,10 +888,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>13</v>
@@ -830,7 +907,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>40</v>
@@ -846,7 +923,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>40</v>
@@ -862,7 +939,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>40</v>
@@ -878,7 +955,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>40</v>
@@ -894,7 +971,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>40</v>
@@ -910,7 +987,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>40</v>
@@ -920,13 +997,13 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="27.95" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>40</v>
@@ -945,7 +1022,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>40</v>
@@ -961,10 +1038,10 @@
         <v>21</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>2</v>
@@ -980,10 +1057,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>13</v>
@@ -993,16 +1070,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>24</v>
@@ -1018,10 +1095,10 @@
         <v>25</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>24</v>
@@ -1037,13 +1114,13 @@
         <v>26</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D26" s="8" t="s">
         <v>40</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="1"/>
       <c r="H26" s="3"/>
@@ -1054,7 +1131,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>40</v>
@@ -1073,7 +1150,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D28" s="8" t="s">
         <v>40</v>
@@ -1089,7 +1166,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>40</v>
@@ -1105,7 +1182,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>40</v>
@@ -1121,7 +1198,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>40</v>
@@ -1137,7 +1214,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>40</v>
@@ -1149,14 +1226,14 @@
     </row>
     <row r="33" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>11</v>
@@ -1172,7 +1249,7 @@
         <v>36</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>40</v>
@@ -1188,7 +1265,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>40</v>
@@ -1204,7 +1281,7 @@
         <v>37</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>40</v>
@@ -1223,7 +1300,7 @@
         <v>35</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>40</v>
@@ -1239,29 +1316,29 @@
         <v>38</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="1"/>
@@ -1275,7 +1352,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>40</v>
@@ -1352,15 +1429,20 @@
   </sheetData>
   <autoFilter ref="B3:G40">
     <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters>
+        <filter val="1"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState ref="B4:F40">
     <sortCondition ref="B4:B40"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="B33" r:id="rId1"/>
+    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>